<commit_message>
unique has to actas imported
</commit_message>
<xml_diff>
--- a/importadores/simcard.xlsx
+++ b/importadores/simcard.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\xampp\htdocs\importadores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp3\htdocs\talentus\importadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369D9DBE-8A58-4451-AF01-C8DB300E5FC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="233">
   <si>
     <t> 89511710100583898662</t>
   </si>
@@ -455,9 +456,6 @@
     <t>89511710120435603565</t>
   </si>
   <si>
-    <t>89511710100583891931</t>
-  </si>
-  <si>
     <t>89511710120488330751</t>
   </si>
   <si>
@@ -491,330 +489,6 @@
     <t>89511710100514626281 </t>
   </si>
   <si>
-    <t> 51977675629</t>
-  </si>
-  <si>
-    <t> 51977701539</t>
-  </si>
-  <si>
-    <t> 51977702722</t>
-  </si>
-  <si>
-    <t> 51977703715</t>
-  </si>
-  <si>
-    <t> 51977704377</t>
-  </si>
-  <si>
-    <t> 51977705156</t>
-  </si>
-  <si>
-    <t> 51977705681</t>
-  </si>
-  <si>
-    <t> 51977691326</t>
-  </si>
-  <si>
-    <t> 51977705302</t>
-  </si>
-  <si>
-    <t> 51977706777</t>
-  </si>
-  <si>
-    <t> 51977700049</t>
-  </si>
-  <si>
-    <t> 51934909279</t>
-  </si>
-  <si>
-    <t> 51934920634</t>
-  </si>
-  <si>
-    <t> 51934914815</t>
-  </si>
-  <si>
-    <t> 51934914695</t>
-  </si>
-  <si>
-    <t> 51923217004</t>
-  </si>
-  <si>
-    <t> 51934912857</t>
-  </si>
-  <si>
-    <t> 51934930122</t>
-  </si>
-  <si>
-    <t> 51934925520</t>
-  </si>
-  <si>
-    <t> 51922825965</t>
-  </si>
-  <si>
-    <t> 51923099153</t>
-  </si>
-  <si>
-    <t> 51922826109</t>
-  </si>
-  <si>
-    <t> 51923358559</t>
-  </si>
-  <si>
-    <t> 51922827944</t>
-  </si>
-  <si>
-    <t> 51923359213</t>
-  </si>
-  <si>
-    <t> 51922826646</t>
-  </si>
-  <si>
-    <t> 51923523449</t>
-  </si>
-  <si>
-    <t> 51923400590</t>
-  </si>
-  <si>
-    <t> 51923360886</t>
-  </si>
-  <si>
-    <t> 51923099999</t>
-  </si>
-  <si>
-    <t> 51919445163</t>
-  </si>
-  <si>
-    <t> 51919445209</t>
-  </si>
-  <si>
-    <t> 51919445204</t>
-  </si>
-  <si>
-    <t> 51919445188</t>
-  </si>
-  <si>
-    <t> 51919445169</t>
-  </si>
-  <si>
-    <t> 51919445159</t>
-  </si>
-  <si>
-    <t> 51919445226</t>
-  </si>
-  <si>
-    <t> 51919445231</t>
-  </si>
-  <si>
-    <t> 51919475520</t>
-  </si>
-  <si>
-    <t> 51919476946</t>
-  </si>
-  <si>
-    <t> 51919477377</t>
-  </si>
-  <si>
-    <t> 51919477365</t>
-  </si>
-  <si>
-    <t> 51923360149</t>
-  </si>
-  <si>
-    <t> 51923357904</t>
-  </si>
-  <si>
-    <t> 51923521288</t>
-  </si>
-  <si>
-    <t> 51923521690</t>
-  </si>
-  <si>
-    <t> 51977698965</t>
-  </si>
-  <si>
-    <t> 51923357154</t>
-  </si>
-  <si>
-    <t> 51934905320</t>
-  </si>
-  <si>
-    <t> 51934924883</t>
-  </si>
-  <si>
-    <t> 51934930413</t>
-  </si>
-  <si>
-    <t> 51924321558</t>
-  </si>
-  <si>
-    <t> 51934931929</t>
-  </si>
-  <si>
-    <t> 51977702293</t>
-  </si>
-  <si>
-    <t> 51919445214</t>
-  </si>
-  <si>
-    <t> 51922825571</t>
-  </si>
-  <si>
-    <t> 51923522954</t>
-  </si>
-  <si>
-    <t> 51977688375</t>
-  </si>
-  <si>
-    <t> 51934924113</t>
-  </si>
-  <si>
-    <t> 51934922317</t>
-  </si>
-  <si>
-    <t> 51977703249</t>
-  </si>
-  <si>
-    <t> 51919445218</t>
-  </si>
-  <si>
-    <t> 51946459370</t>
-  </si>
-  <si>
-    <t> 51946456768</t>
-  </si>
-  <si>
-    <t> 51946462715</t>
-  </si>
-  <si>
-    <t> 51946484533</t>
-  </si>
-  <si>
-    <t> 51946481744</t>
-  </si>
-  <si>
-    <t> 51946469684</t>
-  </si>
-  <si>
-    <t> 51946469328</t>
-  </si>
-  <si>
-    <t> 51946469002</t>
-  </si>
-  <si>
-    <t> 51946466752</t>
-  </si>
-  <si>
-    <t> 51946463719</t>
-  </si>
-  <si>
-    <t> 51946568170</t>
-  </si>
-  <si>
-    <t> 51946444339</t>
-  </si>
-  <si>
-    <t> 51946473367</t>
-  </si>
-  <si>
-    <t> 51946449833</t>
-  </si>
-  <si>
-    <t> 51926923539</t>
-  </si>
-  <si>
-    <t> 51926924273</t>
-  </si>
-  <si>
-    <t> 51926926273</t>
-  </si>
-  <si>
-    <t> 51926926805</t>
-  </si>
-  <si>
-    <t> 51926927323</t>
-  </si>
-  <si>
-    <t> 51926930796</t>
-  </si>
-  <si>
-    <t> 51926931174</t>
-  </si>
-  <si>
-    <t> 51926931371</t>
-  </si>
-  <si>
-    <t> 51926932048</t>
-  </si>
-  <si>
-    <t> 51981462349</t>
-  </si>
-  <si>
-    <t> 51981465188</t>
-  </si>
-  <si>
-    <t> 51981466582</t>
-  </si>
-  <si>
-    <t> 51981467490</t>
-  </si>
-  <si>
-    <t> 51955083676</t>
-  </si>
-  <si>
-    <t> 51955084275</t>
-  </si>
-  <si>
-    <t> 51955084031</t>
-  </si>
-  <si>
-    <t> 51955084568</t>
-  </si>
-  <si>
-    <t> 51955086413</t>
-  </si>
-  <si>
-    <t> 51955086694</t>
-  </si>
-  <si>
-    <t> 51955086511</t>
-  </si>
-  <si>
-    <t> 51955085163</t>
-  </si>
-  <si>
-    <t> 51955084742</t>
-  </si>
-  <si>
-    <t> 51955086046</t>
-  </si>
-  <si>
-    <t> 51919475250</t>
-  </si>
-  <si>
-    <t> 51946222858</t>
-  </si>
-  <si>
-    <t> 51946249131</t>
-  </si>
-  <si>
-    <t> 51946258441</t>
-  </si>
-  <si>
-    <t> 51946289663</t>
-  </si>
-  <si>
-    <t> 51946300345</t>
-  </si>
-  <si>
-    <t> 51946316843</t>
-  </si>
-  <si>
-    <t> 51946329507</t>
-  </si>
-  <si>
-    <t> 51946337089</t>
-  </si>
-  <si>
     <t> 947117853</t>
   </si>
   <si>
@@ -860,41 +534,206 @@
     <t> 946563249</t>
   </si>
   <si>
-    <t>0000000000</t>
-  </si>
-  <si>
-    <t>0000000001</t>
-  </si>
-  <si>
-    <t>0000000002</t>
-  </si>
-  <si>
-    <t>0000000003</t>
-  </si>
-  <si>
-    <t>0000000004</t>
-  </si>
-  <si>
-    <t>0000000005</t>
-  </si>
-  <si>
-    <t>0000000006</t>
-  </si>
-  <si>
-    <t>0000000007</t>
-  </si>
-  <si>
-    <t>0000000008</t>
+    <t> 977675629</t>
+  </si>
+  <si>
+    <t> 977701539</t>
+  </si>
+  <si>
+    <t> 977702722</t>
+  </si>
+  <si>
+    <t> 977703715</t>
+  </si>
+  <si>
+    <t> 977704377</t>
+  </si>
+  <si>
+    <t> 977705156</t>
+  </si>
+  <si>
+    <t> 977705681</t>
+  </si>
+  <si>
+    <t> 977691326</t>
+  </si>
+  <si>
+    <t> 977705302</t>
+  </si>
+  <si>
+    <t> 977706777</t>
+  </si>
+  <si>
+    <t> 977700049</t>
+  </si>
+  <si>
+    <t> 934909279</t>
+  </si>
+  <si>
+    <t> 934920634</t>
+  </si>
+  <si>
+    <t> 934914815</t>
+  </si>
+  <si>
+    <t> 934914695</t>
+  </si>
+  <si>
+    <t> 923217004</t>
+  </si>
+  <si>
+    <t> 946484533</t>
+  </si>
+  <si>
+    <t> 934922317</t>
+  </si>
+  <si>
+    <t> 946289663</t>
+  </si>
+  <si>
+    <t> 946300345</t>
+  </si>
+  <si>
+    <t> 946316843</t>
+  </si>
+  <si>
+    <t> 946329507</t>
+  </si>
+  <si>
+    <t> 946337089</t>
+  </si>
+  <si>
+    <t> 934912857</t>
+  </si>
+  <si>
+    <t> 934930122</t>
+  </si>
+  <si>
+    <t> 934925520</t>
+  </si>
+  <si>
+    <t> 923099153</t>
+  </si>
+  <si>
+    <t> 919445209</t>
+  </si>
+  <si>
+    <t> 919445204</t>
+  </si>
+  <si>
+    <t> 919445188</t>
+  </si>
+  <si>
+    <t> 919445159</t>
+  </si>
+  <si>
+    <t> 919445231</t>
+  </si>
+  <si>
+    <t> 923360149</t>
+  </si>
+  <si>
+    <t> 923521690</t>
+  </si>
+  <si>
+    <t> 977698965</t>
+  </si>
+  <si>
+    <t> 923357154</t>
+  </si>
+  <si>
+    <t> 934905320</t>
+  </si>
+  <si>
+    <t> 934924883</t>
+  </si>
+  <si>
+    <t> 934930413</t>
+  </si>
+  <si>
+    <t> 924321558</t>
+  </si>
+  <si>
+    <t> 977702293</t>
+  </si>
+  <si>
+    <t> 923522954</t>
+  </si>
+  <si>
+    <t> 934924113</t>
+  </si>
+  <si>
+    <t> 977703249</t>
+  </si>
+  <si>
+    <t> 919445218</t>
+  </si>
+  <si>
+    <t> 946459370</t>
+  </si>
+  <si>
+    <t> 946462715</t>
+  </si>
+  <si>
+    <t> 946469684</t>
+  </si>
+  <si>
+    <t> 946469328</t>
+  </si>
+  <si>
+    <t> 946469002</t>
+  </si>
+  <si>
+    <t> 946466752</t>
+  </si>
+  <si>
+    <t> 946568170</t>
+  </si>
+  <si>
+    <t> 946444339</t>
+  </si>
+  <si>
+    <t> 946473367</t>
+  </si>
+  <si>
+    <t> 946449833</t>
+  </si>
+  <si>
+    <t> 926924273</t>
+  </si>
+  <si>
+    <t> 926926273</t>
+  </si>
+  <si>
+    <t> 926927323</t>
+  </si>
+  <si>
+    <t> 955083676</t>
+  </si>
+  <si>
+    <t> 955084275</t>
+  </si>
+  <si>
+    <t> 955086511</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>sim_card</t>
+  </si>
+  <si>
+    <t>operador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1032,6 +871,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1366,7 +1220,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1385,6 +1239,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1418,7 +1277,7 @@
     <cellStyle name="Énfasis6" xfId="36" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="7" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="5" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Millares 2" xfId="41"/>
+    <cellStyle name="Millares 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Neutral" xfId="6" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="13" builtinId="10" customBuiltin="1"/>
@@ -1427,7 +1286,7 @@
     <cellStyle name="Texto explicativo" xfId="14" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="1" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="2" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="40"/>
+    <cellStyle name="Título 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Total" xfId="15" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1705,11 +1564,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C163"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147:XFD147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,652 +1578,652 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" t="s">
+        <v>231</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>152</v>
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>977700740</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="C12" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
+        <v>977700740</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>934920884</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>922825965</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C23" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>922826109</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>923358559</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>922827944</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>923359213</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>922826646</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>923523449</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>923400590</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>923360886</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>923099999</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>919445163</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C34" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>919445169</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>919445226</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>919475520</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>919476946</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>919477377</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>919477365</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C45" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>923357904</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C47" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
+        <v>923521288</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
         <v>923358953</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C49" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+      <c r="C51" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
         <v>977674081</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C52" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>154</v>
+        <v>53</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+      <c r="A57" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
         <v>919475669</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>934931929</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C59" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2372,956 +2231,956 @@
         <v>209</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>919445214</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>922825571</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C62" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>977688375</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C64" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>946456768</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C69" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>946481744</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C71" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>946463719</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C76" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>926923539</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="C81" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>926926805</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C84" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>926930796</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>926931174</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>926931371</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>926932048</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
+        <v>981462349</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <v>981465188</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>981466582</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>981467490</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="C93" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>955084031</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>955084568</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>955086413</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>955086694</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="C99" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>955085163</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>955084742</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="5">
+        <v>955086046</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="C103" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
+        <v>919475250</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
         <v>946273542</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>946222858</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B106" s="2" t="s">
+      <c r="C106" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>946249131</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>946258441</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="C108" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>259</v>
+        <v>187</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>260</v>
+        <v>188</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>261</v>
+        <v>189</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>262</v>
+        <v>190</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="5">
+      <c r="C113" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="5">
         <v>946590270</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="C115" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B116" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="5">
+      <c r="C117" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="5">
         <v>947143570</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="C118" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>267</v>
+        <v>157</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>269</v>
+        <v>159</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>270</v>
+        <v>160</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>271</v>
+        <v>161</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>272</v>
+        <v>162</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C124" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="5">
+      <c r="C125" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="5">
         <v>919475422</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="C126" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>274</v>
+        <v>164</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>275</v>
+        <v>165</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>276</v>
+        <v>166</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>277</v>
+        <v>167</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C130" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="5">
-        <v>926925301</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C131" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
+        <v>926925301</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
         <v>934934080</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B133" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C132" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="7">
+      <c r="C133" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="7">
         <v>934921960</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B134" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="5">
-        <v>934907995</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="C134" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
-        <v>947126180</v>
+        <v>934907995</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
-        <v>934935638</v>
+        <v>947126180</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
-        <v>977704774</v>
+        <v>934935638</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
-        <v>960388303</v>
+        <v>977704774</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
-        <v>960363220</v>
+        <v>960388303</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
-        <v>960401310</v>
+        <v>960363220</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
-        <v>960386507</v>
+        <v>960401310</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
-        <v>970140206</v>
+        <v>960386507</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
-        <v>970137327</v>
+        <v>970140206</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
-        <v>970137415</v>
+        <v>970137327</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
-        <v>970152596</v>
+        <v>970137415</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
-        <v>926931174</v>
+        <v>970152596</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3329,10 +3188,10 @@
         <v>981002723</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3340,10 +3199,10 @@
         <v>960984868</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3351,10 +3210,10 @@
         <v>970150219</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3362,10 +3221,10 @@
         <v>960523019</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3373,145 +3232,133 @@
         <v>972154343</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
-        <v>51960523534</v>
+        <v>960523534</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
-        <v>51960613114</v>
+        <v>960613114</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
-        <v>51960615799</v>
+        <v>960615799</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>970990659</v>
       </c>
-      <c r="B155" s="4" t="s">
-        <v>278</v>
-      </c>
+      <c r="B155" s="4"/>
       <c r="C155" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>972155161</v>
       </c>
-      <c r="B156" s="4" t="s">
-        <v>279</v>
-      </c>
+      <c r="B156" s="4"/>
       <c r="C156" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>972155363</v>
       </c>
-      <c r="B157" s="4" t="s">
-        <v>280</v>
-      </c>
+      <c r="B157" s="4"/>
       <c r="C157" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>972173171</v>
       </c>
-      <c r="B158" s="4" t="s">
-        <v>281</v>
-      </c>
+      <c r="B158" s="4"/>
       <c r="C158" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>960384068</v>
       </c>
-      <c r="B159" s="4" t="s">
-        <v>282</v>
-      </c>
+      <c r="B159" s="4"/>
       <c r="C159" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>934897909</v>
       </c>
-      <c r="B160" s="4" t="s">
-        <v>283</v>
-      </c>
+      <c r="B160" s="4"/>
       <c r="C160" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>284</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="B161" s="4"/>
       <c r="C161" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>285</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="B162" s="4"/>
       <c r="C162" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
-        <v>51960607632</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>286</v>
-      </c>
+        <v>960607632</v>
+      </c>
+      <c r="B163" s="4"/>
       <c r="C163" s="6" t="s">
-        <v>152</v>
-      </c>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="8"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
image sello contratos and hash
</commit_message>
<xml_diff>
--- a/importadores/simcard.xlsx
+++ b/importadores/simcard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp3\htdocs\talentus\importadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F37C1A-09C9-4B47-858A-1ECD1BFCAC07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17AE9A9-74CA-4403-A245-022123A16D6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -973,7 +973,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>